<commit_message>
Adjust phase in timeline for nonroad biofuel potential
</commit_message>
<xml_diff>
--- a/InputData/trans/MPoEFUbVT/Max Perc of Each Fuel Usable by Veh Tech.xlsx
+++ b/InputData/trans/MPoEFUbVT/Max Perc of Each Fuel Usable by Veh Tech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\MPoEFUbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\MPoEFUbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AB6F7F-6703-4EC9-9AC9-D95123198F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FBF57E-9E0A-4861-96FF-003F2EEA3BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <definedName name="max_biodsl">'Max Biofuel Blends'!$A$3</definedName>
     <definedName name="max_biogas">'Max Biofuel Blends'!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -828,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A53" sqref="A53:XFD56"/>
     </sheetView>
   </sheetViews>
@@ -11119,8 +11119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11156,7 +11156,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B6">
         <v>2050</v>
@@ -11177,7 +11177,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B9">
         <v>2050</v>
@@ -11188,7 +11188,7 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -11324,115 +11324,115 @@
       </c>
       <c r="G14">
         <f>_xlfn.FORECAST.LINEAR(G13,$A$7:$B$7,$A$6:$B$6)</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H14">
         <f t="shared" ref="H14:AI14" si="0">_xlfn.FORECAST.LINEAR(H13,$A$7:$B$7,$A$6:$B$6)</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P14">
         <f t="shared" si="0"/>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T14">
         <f t="shared" si="0"/>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U14">
         <f t="shared" si="0"/>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V14">
         <f t="shared" si="0"/>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W14">
         <f t="shared" si="0"/>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X14">
         <f t="shared" si="0"/>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y14">
         <f t="shared" si="0"/>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z14">
         <f t="shared" si="0"/>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA14">
         <f t="shared" si="0"/>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB14">
         <f t="shared" si="0"/>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC14">
         <f t="shared" si="0"/>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD14">
         <f t="shared" si="0"/>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE14">
         <f t="shared" si="0"/>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF14">
         <f t="shared" si="0"/>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG14">
         <f t="shared" si="0"/>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH14">
         <f t="shared" si="0"/>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI14">
         <f t="shared" si="0"/>
@@ -11571,119 +11571,119 @@
       </c>
       <c r="G17" cm="1">
         <f t="array" ref="G17">TREND($A$10:$B$10,$A$9:$B$9,G16)</f>
-        <v>1.7241379310341642E-2</v>
+        <v>3.9999999999992042E-2</v>
       </c>
       <c r="H17" cm="1">
         <f t="array" ref="H17">TREND($A$10:$B$10,$A$9:$B$9,H16)</f>
-        <v>3.448275862069039E-2</v>
+        <v>5.9999999999995168E-2</v>
       </c>
       <c r="I17" cm="1">
         <f t="array" ref="I17">TREND($A$10:$B$10,$A$9:$B$9,I16)</f>
-        <v>5.1724137931032033E-2</v>
+        <v>7.9999999999998295E-2</v>
       </c>
       <c r="J17" cm="1">
         <f t="array" ref="J17">TREND($A$10:$B$10,$A$9:$B$9,J16)</f>
-        <v>6.896551724138078E-2</v>
+        <v>9.9999999999994316E-2</v>
       </c>
       <c r="K17" cm="1">
         <f t="array" ref="K17">TREND($A$10:$B$10,$A$9:$B$9,K16)</f>
-        <v>8.6206896551722423E-2</v>
+        <v>0.11999999999999744</v>
       </c>
       <c r="L17" cm="1">
         <f t="array" ref="L17">TREND($A$10:$B$10,$A$9:$B$9,L16)</f>
-        <v>0.10344827586207117</v>
+        <v>0.13999999999999346</v>
       </c>
       <c r="M17" cm="1">
         <f t="array" ref="M17">TREND($A$10:$B$10,$A$9:$B$9,M16)</f>
-        <v>0.12068965517241281</v>
+        <v>0.15999999999999659</v>
       </c>
       <c r="N17" cm="1">
         <f t="array" ref="N17">TREND($A$10:$B$10,$A$9:$B$9,N16)</f>
-        <v>0.13793103448275446</v>
+        <v>0.17999999999999261</v>
       </c>
       <c r="O17" cm="1">
         <f t="array" ref="O17">TREND($A$10:$B$10,$A$9:$B$9,O16)</f>
-        <v>0.1551724137931032</v>
+        <v>0.19999999999999574</v>
       </c>
       <c r="P17" cm="1">
         <f t="array" ref="P17">TREND($A$10:$B$10,$A$9:$B$9,P16)</f>
-        <v>0.17241379310344485</v>
+        <v>0.21999999999999176</v>
       </c>
       <c r="Q17" cm="1">
         <f t="array" ref="Q17">TREND($A$10:$B$10,$A$9:$B$9,Q16)</f>
-        <v>0.18965517241379359</v>
+        <v>0.23999999999999488</v>
       </c>
       <c r="R17" cm="1">
         <f t="array" ref="R17">TREND($A$10:$B$10,$A$9:$B$9,R16)</f>
-        <v>0.20689655172413524</v>
+        <v>0.25999999999999801</v>
       </c>
       <c r="S17" cm="1">
         <f t="array" ref="S17">TREND($A$10:$B$10,$A$9:$B$9,S16)</f>
-        <v>0.22413793103448398</v>
+        <v>0.27999999999999403</v>
       </c>
       <c r="T17" cm="1">
         <f t="array" ref="T17">TREND($A$10:$B$10,$A$9:$B$9,T16)</f>
-        <v>0.24137931034482563</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="U17" cm="1">
         <f t="array" ref="U17">TREND($A$10:$B$10,$A$9:$B$9,U16)</f>
-        <v>0.25862068965517437</v>
+        <v>0.31999999999999318</v>
       </c>
       <c r="V17" cm="1">
         <f t="array" ref="V17">TREND($A$10:$B$10,$A$9:$B$9,V16)</f>
-        <v>0.27586206896551602</v>
+        <v>0.33999999999999631</v>
       </c>
       <c r="W17" cm="1">
         <f t="array" ref="W17">TREND($A$10:$B$10,$A$9:$B$9,W16)</f>
-        <v>0.29310344827586476</v>
+        <v>0.35999999999999233</v>
       </c>
       <c r="X17" cm="1">
         <f t="array" ref="X17">TREND($A$10:$B$10,$A$9:$B$9,X16)</f>
-        <v>0.31034482758620641</v>
+        <v>0.37999999999999545</v>
       </c>
       <c r="Y17" cm="1">
         <f t="array" ref="Y17">TREND($A$10:$B$10,$A$9:$B$9,Y16)</f>
-        <v>0.32758620689654805</v>
+        <v>0.39999999999999858</v>
       </c>
       <c r="Z17" cm="1">
         <f t="array" ref="Z17">TREND($A$10:$B$10,$A$9:$B$9,Z16)</f>
-        <v>0.3448275862068968</v>
+        <v>0.4199999999999946</v>
       </c>
       <c r="AA17" cm="1">
         <f t="array" ref="AA17">TREND($A$10:$B$10,$A$9:$B$9,AA16)</f>
-        <v>0.36206896551723844</v>
+        <v>0.43999999999999773</v>
       </c>
       <c r="AB17" cm="1">
         <f t="array" ref="AB17">TREND($A$10:$B$10,$A$9:$B$9,AB16)</f>
-        <v>0.37931034482758719</v>
+        <v>0.45999999999999375</v>
       </c>
       <c r="AC17" cm="1">
         <f t="array" ref="AC17">TREND($A$10:$B$10,$A$9:$B$9,AC16)</f>
-        <v>0.39655172413792883</v>
+        <v>0.47999999999999687</v>
       </c>
       <c r="AD17" cm="1">
         <f t="array" ref="AD17">TREND($A$10:$B$10,$A$9:$B$9,AD16)</f>
-        <v>0.41379310344827758</v>
+        <v>0.49999999999999289</v>
       </c>
       <c r="AE17" cm="1">
         <f t="array" ref="AE17">TREND($A$10:$B$10,$A$9:$B$9,AE16)</f>
-        <v>0.43103448275861922</v>
+        <v>0.51999999999999602</v>
       </c>
       <c r="AF17" cm="1">
         <f t="array" ref="AF17">TREND($A$10:$B$10,$A$9:$B$9,AF16)</f>
-        <v>0.44827586206896797</v>
+        <v>0.53999999999999204</v>
       </c>
       <c r="AG17" cm="1">
         <f t="array" ref="AG17">TREND($A$10:$B$10,$A$9:$B$9,AG16)</f>
-        <v>0.46551724137930961</v>
+        <v>0.55999999999999517</v>
       </c>
       <c r="AH17" cm="1">
         <f t="array" ref="AH17">TREND($A$10:$B$10,$A$9:$B$9,AH16)</f>
-        <v>0.48275862068965125</v>
+        <v>0.57999999999999829</v>
       </c>
       <c r="AI17" cm="1">
         <f t="array" ref="AI17">TREND($A$10:$B$10,$A$9:$B$9,AI16)</f>
-        <v>0.5</v>
+        <v>0.59999999999999432</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
@@ -32148,115 +32148,115 @@
       </c>
       <c r="G6">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H6">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I6">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J6">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K6">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L6">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M6">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N6">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O6">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P6">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q6">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R6">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S6">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T6">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V6">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W6">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X6">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y6">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z6">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA6">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB6">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC6">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD6">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE6">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF6">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG6">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH6">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI6">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -33487,115 +33487,115 @@
       </c>
       <c r="G7">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H7">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I7">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J7">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K7">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L7">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M7">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N7">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O7">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P7">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q7">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R7">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S7">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T7">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U7">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V7">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W7">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X7">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y7">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z7">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA7">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB7">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC7">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD7">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE7">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF7">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG7">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH7">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI7">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -39442,115 +39442,115 @@
       </c>
       <c r="G6">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H6">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I6">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J6">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K6">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L6">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M6">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N6">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O6">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P6">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q6">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R6">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S6">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T6">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V6">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W6">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X6">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y6">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z6">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA6">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB6">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC6">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD6">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE6">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF6">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG6">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH6">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI6">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -40779,115 +40779,115 @@
       </c>
       <c r="G7">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H7">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I7">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J7">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K7">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L7">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M7">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N7">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O7">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P7">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q7">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R7">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S7">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T7">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U7">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V7">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W7">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X7">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y7">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z7">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA7">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB7">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC7">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD7">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE7">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF7">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG7">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH7">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI7">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -46734,115 +46734,115 @@
       </c>
       <c r="G6">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H6">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I6">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J6">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K6">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L6">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M6">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N6">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O6">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P6">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q6">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R6">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S6">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T6">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V6">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W6">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X6">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y6">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z6">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA6">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB6">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC6">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD6">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE6">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF6">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG6">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH6">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI6">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -48071,115 +48071,115 @@
       </c>
       <c r="G7">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H7">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I7">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J7">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K7">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L7">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M7">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N7">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O7">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P7">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q7">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R7">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S7">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T7">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U7">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V7">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W7">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X7">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y7">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z7">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA7">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB7">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC7">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD7">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE7">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF7">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG7">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH7">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI7">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -52797,115 +52797,115 @@
       </c>
       <c r="G6">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H6">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I6">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J6">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K6">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L6">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M6">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N6">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O6">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P6">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q6">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R6">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S6">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T6">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V6">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W6">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X6">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y6">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z6">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA6">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB6">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC6">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD6">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE6">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF6">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG6">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH6">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI6">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -54134,115 +54134,115 @@
       </c>
       <c r="G7">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H7">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I7">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J7">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K7">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L7">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M7">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N7">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O7">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P7">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q7">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R7">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S7">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T7">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U7">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V7">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W7">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X7">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y7">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z7">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA7">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB7">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC7">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD7">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE7">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF7">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG7">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH7">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI7">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -60126,115 +60126,115 @@
       </c>
       <c r="G6">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H6">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I6">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J6">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K6">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L6">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M6">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N6">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O6">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P6">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q6">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R6">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S6">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T6">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V6">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W6">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X6">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y6">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z6">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA6">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB6">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC6">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD6">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE6">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF6">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG6">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH6">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI6">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -61463,115 +61463,115 @@
       </c>
       <c r="G7">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H7">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I7">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J7">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K7">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L7">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M7">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N7">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O7">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P7">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q7">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R7">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S7">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T7">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U7">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V7">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W7">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X7">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y7">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z7">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA7">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB7">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC7">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD7">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE7">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF7">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG7">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH7">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI7">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -66189,115 +66189,115 @@
       </c>
       <c r="G6">
         <f>'Max Biofuel Blends'!G$14</f>
-        <v>3.4482758620683285E-2</v>
+        <v>6.6666666666677088E-2</v>
       </c>
       <c r="H6">
         <f>'Max Biofuel Blends'!H$14</f>
-        <v>6.896551724138078E-2</v>
+        <v>0.10000000000000853</v>
       </c>
       <c r="I6">
         <f>'Max Biofuel Blends'!I$14</f>
-        <v>0.10344827586206407</v>
+        <v>0.13333333333333997</v>
       </c>
       <c r="J6">
         <f>'Max Biofuel Blends'!J$14</f>
-        <v>0.13793103448276156</v>
+        <v>0.1666666666666714</v>
       </c>
       <c r="K6">
         <f>'Max Biofuel Blends'!K$14</f>
-        <v>0.17241379310344485</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="L6">
         <f>'Max Biofuel Blends'!L$14</f>
-        <v>0.20689655172414234</v>
+        <v>0.23333333333333428</v>
       </c>
       <c r="M6">
         <f>'Max Biofuel Blends'!M$14</f>
-        <v>0.24137931034482563</v>
+        <v>0.26666666666666572</v>
       </c>
       <c r="N6">
         <f>'Max Biofuel Blends'!N$14</f>
-        <v>0.27586206896550891</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="O6">
         <f>'Max Biofuel Blends'!O$14</f>
-        <v>0.31034482758620641</v>
+        <v>0.33333333333334281</v>
       </c>
       <c r="P6">
         <f>'Max Biofuel Blends'!P$14</f>
-        <v>0.34482758620688969</v>
+        <v>0.36666666666667425</v>
       </c>
       <c r="Q6">
         <f>'Max Biofuel Blends'!Q$14</f>
-        <v>0.37931034482758719</v>
+        <v>0.40000000000000568</v>
       </c>
       <c r="R6">
         <f>'Max Biofuel Blends'!R$14</f>
-        <v>0.41379310344827047</v>
+        <v>0.43333333333333712</v>
       </c>
       <c r="S6">
         <f>'Max Biofuel Blends'!S$14</f>
-        <v>0.44827586206896797</v>
+        <v>0.46666666666666856</v>
       </c>
       <c r="T6">
         <f>'Max Biofuel Blends'!T$14</f>
-        <v>0.48275862068965125</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
         <f>'Max Biofuel Blends'!U$14</f>
-        <v>0.51724137931034875</v>
+        <v>0.53333333333333144</v>
       </c>
       <c r="V6">
         <f>'Max Biofuel Blends'!V$14</f>
-        <v>0.55172413793103203</v>
+        <v>0.56666666666667709</v>
       </c>
       <c r="W6">
         <f>'Max Biofuel Blends'!W$14</f>
-        <v>0.58620689655172953</v>
+        <v>0.60000000000000853</v>
       </c>
       <c r="X6">
         <f>'Max Biofuel Blends'!X$14</f>
-        <v>0.62068965517241281</v>
+        <v>0.63333333333333997</v>
       </c>
       <c r="Y6">
         <f>'Max Biofuel Blends'!Y$14</f>
-        <v>0.6551724137930961</v>
+        <v>0.6666666666666714</v>
       </c>
       <c r="Z6">
         <f>'Max Biofuel Blends'!Z$14</f>
-        <v>0.68965517241379359</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="AA6">
         <f>'Max Biofuel Blends'!AA$14</f>
-        <v>0.72413793103447688</v>
+        <v>0.73333333333333428</v>
       </c>
       <c r="AB6">
         <f>'Max Biofuel Blends'!AB$14</f>
-        <v>0.75862068965517437</v>
+        <v>0.76666666666666572</v>
       </c>
       <c r="AC6">
         <f>'Max Biofuel Blends'!AC$14</f>
-        <v>0.79310344827585766</v>
+        <v>0.79999999999999716</v>
       </c>
       <c r="AD6">
         <f>'Max Biofuel Blends'!AD$14</f>
-        <v>0.82758620689655515</v>
+        <v>0.83333333333334281</v>
       </c>
       <c r="AE6">
         <f>'Max Biofuel Blends'!AE$14</f>
-        <v>0.86206896551723844</v>
+        <v>0.86666666666667425</v>
       </c>
       <c r="AF6">
         <f>'Max Biofuel Blends'!AF$14</f>
-        <v>0.89655172413793593</v>
+        <v>0.90000000000000568</v>
       </c>
       <c r="AG6">
         <f>'Max Biofuel Blends'!AG$14</f>
-        <v>0.93103448275861922</v>
+        <v>0.93333333333333712</v>
       </c>
       <c r="AH6">
         <f>'Max Biofuel Blends'!AH$14</f>
-        <v>0.9655172413793025</v>
+        <v>0.96666666666666856</v>
       </c>
       <c r="AI6">
         <f>'Max Biofuel Blends'!AI$14</f>
@@ -66851,8 +66851,8 @@
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AI7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67528,119 +67528,119 @@
       </c>
       <c r="G7">
         <f>'Max Biofuel Blends'!G$17</f>
-        <v>1.7241379310341642E-2</v>
+        <v>3.9999999999992042E-2</v>
       </c>
       <c r="H7">
         <f>'Max Biofuel Blends'!H$17</f>
-        <v>3.448275862069039E-2</v>
+        <v>5.9999999999995168E-2</v>
       </c>
       <c r="I7">
         <f>'Max Biofuel Blends'!I$17</f>
-        <v>5.1724137931032033E-2</v>
+        <v>7.9999999999998295E-2</v>
       </c>
       <c r="J7">
         <f>'Max Biofuel Blends'!J$17</f>
-        <v>6.896551724138078E-2</v>
+        <v>9.9999999999994316E-2</v>
       </c>
       <c r="K7">
         <f>'Max Biofuel Blends'!K$17</f>
-        <v>8.6206896551722423E-2</v>
+        <v>0.11999999999999744</v>
       </c>
       <c r="L7">
         <f>'Max Biofuel Blends'!L$17</f>
-        <v>0.10344827586207117</v>
+        <v>0.13999999999999346</v>
       </c>
       <c r="M7">
         <f>'Max Biofuel Blends'!M$17</f>
-        <v>0.12068965517241281</v>
+        <v>0.15999999999999659</v>
       </c>
       <c r="N7">
         <f>'Max Biofuel Blends'!N$17</f>
-        <v>0.13793103448275446</v>
+        <v>0.17999999999999261</v>
       </c>
       <c r="O7">
         <f>'Max Biofuel Blends'!O$17</f>
-        <v>0.1551724137931032</v>
+        <v>0.19999999999999574</v>
       </c>
       <c r="P7">
         <f>'Max Biofuel Blends'!P$17</f>
-        <v>0.17241379310344485</v>
+        <v>0.21999999999999176</v>
       </c>
       <c r="Q7">
         <f>'Max Biofuel Blends'!Q$17</f>
-        <v>0.18965517241379359</v>
+        <v>0.23999999999999488</v>
       </c>
       <c r="R7">
         <f>'Max Biofuel Blends'!R$17</f>
-        <v>0.20689655172413524</v>
+        <v>0.25999999999999801</v>
       </c>
       <c r="S7">
         <f>'Max Biofuel Blends'!S$17</f>
-        <v>0.22413793103448398</v>
+        <v>0.27999999999999403</v>
       </c>
       <c r="T7">
         <f>'Max Biofuel Blends'!T$17</f>
-        <v>0.24137931034482563</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="U7">
         <f>'Max Biofuel Blends'!U$17</f>
-        <v>0.25862068965517437</v>
+        <v>0.31999999999999318</v>
       </c>
       <c r="V7">
         <f>'Max Biofuel Blends'!V$17</f>
-        <v>0.27586206896551602</v>
+        <v>0.33999999999999631</v>
       </c>
       <c r="W7">
         <f>'Max Biofuel Blends'!W$17</f>
-        <v>0.29310344827586476</v>
+        <v>0.35999999999999233</v>
       </c>
       <c r="X7">
         <f>'Max Biofuel Blends'!X$17</f>
-        <v>0.31034482758620641</v>
+        <v>0.37999999999999545</v>
       </c>
       <c r="Y7">
         <f>'Max Biofuel Blends'!Y$17</f>
-        <v>0.32758620689654805</v>
+        <v>0.39999999999999858</v>
       </c>
       <c r="Z7">
         <f>'Max Biofuel Blends'!Z$17</f>
-        <v>0.3448275862068968</v>
+        <v>0.4199999999999946</v>
       </c>
       <c r="AA7">
         <f>'Max Biofuel Blends'!AA$17</f>
-        <v>0.36206896551723844</v>
+        <v>0.43999999999999773</v>
       </c>
       <c r="AB7">
         <f>'Max Biofuel Blends'!AB$17</f>
-        <v>0.37931034482758719</v>
+        <v>0.45999999999999375</v>
       </c>
       <c r="AC7">
         <f>'Max Biofuel Blends'!AC$17</f>
-        <v>0.39655172413792883</v>
+        <v>0.47999999999999687</v>
       </c>
       <c r="AD7">
         <f>'Max Biofuel Blends'!AD$17</f>
-        <v>0.41379310344827758</v>
+        <v>0.49999999999999289</v>
       </c>
       <c r="AE7">
         <f>'Max Biofuel Blends'!AE$17</f>
-        <v>0.43103448275861922</v>
+        <v>0.51999999999999602</v>
       </c>
       <c r="AF7">
         <f>'Max Biofuel Blends'!AF$17</f>
-        <v>0.44827586206896797</v>
+        <v>0.53999999999999204</v>
       </c>
       <c r="AG7">
         <f>'Max Biofuel Blends'!AG$17</f>
-        <v>0.46551724137930961</v>
+        <v>0.55999999999999517</v>
       </c>
       <c r="AH7">
         <f>'Max Biofuel Blends'!AH$17</f>
-        <v>0.48275862068965125</v>
+        <v>0.57999999999999829</v>
       </c>
       <c r="AI7">
         <f>'Max Biofuel Blends'!AI$17</f>
-        <v>0.5</v>
+        <v>0.59999999999999432</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">

</xml_diff>